<commit_message>
PROS-12268 add Oral Care Eye level
</commit_message>
<xml_diff>
--- a/Projects/PNGCN_PROD/Data/pngcn_variant_block_template_v1.xlsx
+++ b/Projects/PNGCN_PROD/Data/pngcn_variant_block_template_v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">KPI_NAME</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">Safeguard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crest</t>
   </si>
 </sst>
 </file>
@@ -56,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,6 +88,12 @@
       <sz val="10.5"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -132,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -142,6 +154,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,21 +178,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,6 +229,23 @@
         <v>3</v>
       </c>
       <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>